<commit_message>
Add meeting minutes and worklogs
</commit_message>
<xml_diff>
--- a/Worklog.xlsx
+++ b/Worklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SIT723\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0D47EC-931A-40D9-AC0C-E7686FDC12AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFED52F-5203-41A4-A15D-122037D0F70A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D01C876E-0C57-1449-A864-F752FD507052}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D01C876E-0C57-1449-A864-F752FD507052}"/>
   </bookViews>
   <sheets>
     <sheet name="Logs" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="78">
   <si>
     <t>Student Name</t>
   </si>
@@ -248,6 +248,27 @@
   </si>
   <si>
     <t xml:space="preserve">Completing Task 4.1P </t>
+  </si>
+  <si>
+    <t>Week 5 meeting with superviors</t>
+  </si>
+  <si>
+    <t>Integrate the MobileNet with FER2013</t>
+  </si>
+  <si>
+    <t>Hypertune the experiment of MobileNet with FER2013 and generate results</t>
+  </si>
+  <si>
+    <t>Find pre-processing and parameter tuning techniques in good papers</t>
+  </si>
+  <si>
+    <t>Locate CK+ dataset and manipluate the preprocessing</t>
+  </si>
+  <si>
+    <t>Experiment ResNet20 with CK+ dataset</t>
+  </si>
+  <si>
+    <t>Work task 5.1P</t>
   </si>
 </sst>
 </file>
@@ -685,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC54600-A529-144A-8AA1-058C0E013D1F}">
-  <dimension ref="A1:H249"/>
+  <dimension ref="A1:H250"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1993,75 +2014,455 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D57" s="4"/>
+      <c r="A57" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" s="4">
+        <v>44417</v>
+      </c>
+      <c r="E57">
+        <v>60</v>
+      </c>
+      <c r="F57" t="s">
+        <v>15</v>
+      </c>
+      <c r="G57" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D58" s="4"/>
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="4">
+        <v>44417</v>
+      </c>
+      <c r="E58">
+        <v>120</v>
+      </c>
+      <c r="F58" t="s">
+        <v>20</v>
+      </c>
+      <c r="G58" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D59" s="4"/>
+      <c r="A59" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="4">
+        <v>44417</v>
+      </c>
+      <c r="E59">
+        <v>60</v>
+      </c>
+      <c r="F59" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D60" s="4"/>
+      <c r="A60" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="4">
+        <v>44418</v>
+      </c>
+      <c r="E60">
+        <v>120</v>
+      </c>
+      <c r="F60" t="s">
+        <v>20</v>
+      </c>
+      <c r="G60" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D61" s="4"/>
+      <c r="A61" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="4">
+        <v>44418</v>
+      </c>
+      <c r="E61">
+        <v>120</v>
+      </c>
+      <c r="F61" t="s">
+        <v>20</v>
+      </c>
+      <c r="G61" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D62" s="4"/>
+      <c r="A62" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" s="4">
+        <v>44418</v>
+      </c>
+      <c r="E62">
+        <v>80</v>
+      </c>
+      <c r="F62" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D63" s="4"/>
+      <c r="A63" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" s="4">
+        <v>44419</v>
+      </c>
+      <c r="E63">
+        <v>120</v>
+      </c>
+      <c r="F63" t="s">
+        <v>20</v>
+      </c>
+      <c r="G63" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D64" s="4"/>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="4"/>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" s="4"/>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" s="4"/>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68" s="4"/>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" s="4"/>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" s="4"/>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" s="4"/>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72" s="4"/>
-    </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D73" s="4"/>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D74" s="4"/>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="4"/>
-    </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" s="4">
+        <v>44419</v>
+      </c>
+      <c r="E64">
+        <v>120</v>
+      </c>
+      <c r="F64" t="s">
+        <v>20</v>
+      </c>
+      <c r="G64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" s="4">
+        <v>44419</v>
+      </c>
+      <c r="E65">
+        <v>120</v>
+      </c>
+      <c r="F65" t="s">
+        <v>20</v>
+      </c>
+      <c r="G65" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" t="s">
+        <v>25</v>
+      </c>
+      <c r="D66" s="4">
+        <v>44421</v>
+      </c>
+      <c r="E66">
+        <v>120</v>
+      </c>
+      <c r="F66" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D67" s="4">
+        <v>44421</v>
+      </c>
+      <c r="E67">
+        <v>120</v>
+      </c>
+      <c r="F67" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" s="4">
+        <v>44421</v>
+      </c>
+      <c r="E68">
+        <v>90</v>
+      </c>
+      <c r="F68" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" t="s">
+        <v>25</v>
+      </c>
+      <c r="D69" s="4">
+        <v>44422</v>
+      </c>
+      <c r="E69">
+        <v>120</v>
+      </c>
+      <c r="F69" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" s="4">
+        <v>44422</v>
+      </c>
+      <c r="E70">
+        <v>120</v>
+      </c>
+      <c r="F70" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" t="s">
+        <v>24</v>
+      </c>
+      <c r="C71" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71" s="4">
+        <v>44422</v>
+      </c>
+      <c r="E71">
+        <v>40</v>
+      </c>
+      <c r="F71" t="s">
+        <v>20</v>
+      </c>
+      <c r="G71" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72" s="4">
+        <v>44423</v>
+      </c>
+      <c r="E72">
+        <v>120</v>
+      </c>
+      <c r="F72" t="s">
+        <v>20</v>
+      </c>
+      <c r="G72" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" t="s">
+        <v>25</v>
+      </c>
+      <c r="D73" s="4">
+        <v>44423</v>
+      </c>
+      <c r="E73">
+        <v>120</v>
+      </c>
+      <c r="F73" t="s">
+        <v>20</v>
+      </c>
+      <c r="G73" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" s="4">
+        <v>44423</v>
+      </c>
+      <c r="E74">
+        <v>110</v>
+      </c>
+      <c r="F74" t="s">
+        <v>20</v>
+      </c>
+      <c r="G74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" t="s">
+        <v>25</v>
+      </c>
+      <c r="D75" s="4">
+        <v>44423</v>
+      </c>
+      <c r="E75">
+        <v>120</v>
+      </c>
+      <c r="F75" t="s">
+        <v>16</v>
+      </c>
+      <c r="G75" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D77" s="4"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D79" s="4"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D80" s="4"/>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
@@ -2570,6 +2971,9 @@
     </row>
     <row r="249" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D249" s="4"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D250" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2581,7 +2985,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E439</xm:sqref>
+          <xm:sqref>E3:E440</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A18E5B6F-7CCC-C74F-9785-6997C435583D}">
           <x14:formula1>
@@ -2599,8 +3003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE2447B-8FF1-4200-A439-D9EB41D71D4F}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2680,8 +3084,14 @@
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="5">
+        <f>ROUNDDOWN(SUM(Logs!E57:E75)/60,0)</f>
+        <v>33</v>
+      </c>
+      <c r="C7" s="5">
+        <f>MOD(SUM(Logs!E57:E75),60)</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -2737,12 +3147,12 @@
         <v>61</v>
       </c>
       <c r="B15" s="5">
-        <f>ROUNDDOWN(SUM(Logs!E3:E200)/60,0)</f>
-        <v>96</v>
+        <f>ROUNDDOWN(SUM(Logs!E3:E201)/60,0)</f>
+        <v>129</v>
       </c>
       <c r="C15" s="5">
-        <f>MOD(SUM(Logs!E3:E200),60)</f>
-        <v>30</v>
+        <f>MOD(SUM(Logs!E3:E201),60)</f>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2870,6 +3280,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010082532935BEA4414DAD83A5DF5EC08D50" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1fab9b1b639c92c05cfd4aa2b4bf08c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffdfa1cc-c946-49f6-99ef-ff4ab350a4c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cad3acc22b2eb44b3a116b77879253d7" ns2:_="">
     <xsd:import namespace="ffdfa1cc-c946-49f6-99ef-ff4ab350a4c7"/>
@@ -3001,12 +3417,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3017,6 +3427,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C84895-33C6-4EEF-ADE3-B2C6A0E7CE9B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FF34756-59E0-48B0-8E6C-773EF7EF3DA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3034,15 +3453,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C84895-33C6-4EEF-ADE3-B2C6A0E7CE9B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F33CB9-EBB9-4740-8AC2-6F0A2CE058F7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update worklog and meeting minutes
</commit_message>
<xml_diff>
--- a/Worklog.xlsx
+++ b/Worklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SIT723\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FB6791-AB40-43A9-BE15-311C97E1EC2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168B57DE-E359-4198-B246-E9DFEFBB4131}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D01C876E-0C57-1449-A864-F752FD507052}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D01C876E-0C57-1449-A864-F752FD507052}"/>
   </bookViews>
   <sheets>
     <sheet name="Logs" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="92">
   <si>
     <t>Student Name</t>
   </si>
@@ -293,6 +293,24 @@
   </si>
   <si>
     <t>Task 6.1</t>
+  </si>
+  <si>
+    <t>Prepare detail report on experiment</t>
+  </si>
+  <si>
+    <t>Re-design the codes for model save and reload to extend cross folding validation to 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search for detail of Real-time and preprocess data augmentation and select the most benefitical on for conducting experiment </t>
+  </si>
+  <si>
+    <t>Conduct experiment using 10 folds cross validation (CBAM + ResNet, SDG, learing rate 0.1, 0.05, 0.001)</t>
+  </si>
+  <si>
+    <t>Conduct experiment using 10 folds cross validation (CBAM + ResNet, Adam, learing rate 0.01, 0.001, 0.0001)</t>
+  </si>
+  <si>
+    <t>Task 7.1</t>
   </si>
 </sst>
 </file>
@@ -732,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC54600-A529-144A-8AA1-058C0E013D1F}">
   <dimension ref="A1:H250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D92" workbookViewId="0">
-      <selection activeCell="G97" sqref="G97"/>
+    <sheetView topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3211,66 +3229,346 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D108" s="4"/>
+      <c r="A108" t="s">
+        <v>23</v>
+      </c>
+      <c r="B108" t="s">
+        <v>24</v>
+      </c>
+      <c r="C108" t="s">
+        <v>25</v>
+      </c>
+      <c r="D108" s="4">
+        <v>44439</v>
+      </c>
+      <c r="E108">
+        <v>110</v>
+      </c>
+      <c r="F108" t="s">
+        <v>20</v>
+      </c>
+      <c r="G108" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D109" s="4"/>
+      <c r="A109" t="s">
+        <v>23</v>
+      </c>
+      <c r="B109" t="s">
+        <v>24</v>
+      </c>
+      <c r="C109" t="s">
+        <v>25</v>
+      </c>
+      <c r="D109" s="4">
+        <v>44440</v>
+      </c>
+      <c r="E109">
+        <v>100</v>
+      </c>
+      <c r="F109" t="s">
+        <v>20</v>
+      </c>
+      <c r="G109" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D110" s="4"/>
+      <c r="A110" t="s">
+        <v>23</v>
+      </c>
+      <c r="B110" t="s">
+        <v>24</v>
+      </c>
+      <c r="C110" t="s">
+        <v>25</v>
+      </c>
+      <c r="D110" s="4">
+        <v>44441</v>
+      </c>
+      <c r="E110">
+        <v>120</v>
+      </c>
+      <c r="F110" t="s">
+        <v>12</v>
+      </c>
+      <c r="G110" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D111" s="4"/>
+      <c r="A111" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" t="s">
+        <v>24</v>
+      </c>
+      <c r="C111" t="s">
+        <v>25</v>
+      </c>
+      <c r="D111" s="4">
+        <v>44442</v>
+      </c>
+      <c r="E111">
+        <v>120</v>
+      </c>
+      <c r="F111" t="s">
+        <v>20</v>
+      </c>
+      <c r="G111" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D112" s="4"/>
-    </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D113" s="4"/>
-    </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D114" s="4"/>
-    </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D115" s="4"/>
-    </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D116" s="4"/>
-    </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D117" s="4"/>
-    </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D118" s="4"/>
-    </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D119" s="4"/>
-    </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D120" s="4"/>
-    </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D121" s="4"/>
-    </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" t="s">
+        <v>24</v>
+      </c>
+      <c r="C112" t="s">
+        <v>25</v>
+      </c>
+      <c r="D112" s="4">
+        <v>44442</v>
+      </c>
+      <c r="E112">
+        <v>120</v>
+      </c>
+      <c r="F112" t="s">
+        <v>20</v>
+      </c>
+      <c r="G112" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>23</v>
+      </c>
+      <c r="B113" t="s">
+        <v>24</v>
+      </c>
+      <c r="C113" t="s">
+        <v>25</v>
+      </c>
+      <c r="D113" s="4">
+        <v>44442</v>
+      </c>
+      <c r="E113">
+        <v>120</v>
+      </c>
+      <c r="F113" t="s">
+        <v>20</v>
+      </c>
+      <c r="G113" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" t="s">
+        <v>24</v>
+      </c>
+      <c r="C114" t="s">
+        <v>25</v>
+      </c>
+      <c r="D114" s="4">
+        <v>44442</v>
+      </c>
+      <c r="E114">
+        <v>120</v>
+      </c>
+      <c r="F114" t="s">
+        <v>20</v>
+      </c>
+      <c r="G114" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>23</v>
+      </c>
+      <c r="B115" t="s">
+        <v>24</v>
+      </c>
+      <c r="C115" t="s">
+        <v>25</v>
+      </c>
+      <c r="D115" s="4">
+        <v>44442</v>
+      </c>
+      <c r="E115">
+        <v>90</v>
+      </c>
+      <c r="F115" t="s">
+        <v>20</v>
+      </c>
+      <c r="G115" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>23</v>
+      </c>
+      <c r="B116" t="s">
+        <v>24</v>
+      </c>
+      <c r="C116" t="s">
+        <v>25</v>
+      </c>
+      <c r="D116" s="4">
+        <v>44443</v>
+      </c>
+      <c r="E116">
+        <v>120</v>
+      </c>
+      <c r="F116" t="s">
+        <v>20</v>
+      </c>
+      <c r="G116" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" t="s">
+        <v>24</v>
+      </c>
+      <c r="C117" t="s">
+        <v>25</v>
+      </c>
+      <c r="D117" s="4">
+        <v>44443</v>
+      </c>
+      <c r="E117">
+        <v>120</v>
+      </c>
+      <c r="F117" t="s">
+        <v>20</v>
+      </c>
+      <c r="G117" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>23</v>
+      </c>
+      <c r="B118" t="s">
+        <v>24</v>
+      </c>
+      <c r="C118" t="s">
+        <v>25</v>
+      </c>
+      <c r="D118" s="4">
+        <v>44443</v>
+      </c>
+      <c r="E118">
+        <v>120</v>
+      </c>
+      <c r="F118" t="s">
+        <v>20</v>
+      </c>
+      <c r="G118" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>23</v>
+      </c>
+      <c r="B119" t="s">
+        <v>24</v>
+      </c>
+      <c r="C119" t="s">
+        <v>25</v>
+      </c>
+      <c r="D119" s="4">
+        <v>44443</v>
+      </c>
+      <c r="E119">
+        <v>120</v>
+      </c>
+      <c r="F119" t="s">
+        <v>20</v>
+      </c>
+      <c r="G119" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>23</v>
+      </c>
+      <c r="B120" t="s">
+        <v>24</v>
+      </c>
+      <c r="C120" t="s">
+        <v>25</v>
+      </c>
+      <c r="D120" s="4">
+        <v>44443</v>
+      </c>
+      <c r="E120">
+        <v>110</v>
+      </c>
+      <c r="F120" t="s">
+        <v>20</v>
+      </c>
+      <c r="G120" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>23</v>
+      </c>
+      <c r="B121" t="s">
+        <v>24</v>
+      </c>
+      <c r="C121" t="s">
+        <v>25</v>
+      </c>
+      <c r="D121" s="4">
+        <v>44444</v>
+      </c>
+      <c r="E121">
+        <v>90</v>
+      </c>
+      <c r="F121" t="s">
+        <v>16</v>
+      </c>
+      <c r="G121" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D122" s="4"/>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D123" s="4"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D124" s="4"/>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D125" s="4"/>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D126" s="4"/>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D127" s="4"/>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D128" s="4"/>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.25">
@@ -3667,8 +3965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE2447B-8FF1-4200-A439-D9EB41D71D4F}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3787,8 +4085,14 @@
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="5">
+        <f>ROUNDDOWN(SUM(Logs!E108:E121)/60,0)</f>
+        <v>26</v>
+      </c>
+      <c r="C10" s="5">
+        <f>MOD(SUM(Logs!E108:E121),60)</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -3824,11 +4128,11 @@
       </c>
       <c r="B15" s="5">
         <f>ROUNDDOWN(SUM(Logs!E3:E201)/60,0)</f>
-        <v>187</v>
+        <v>213</v>
       </c>
       <c r="C15" s="5">
         <f>MOD(SUM(Logs!E3:E201),60)</f>
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -3956,6 +4260,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010082532935BEA4414DAD83A5DF5EC08D50" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1fab9b1b639c92c05cfd4aa2b4bf08c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffdfa1cc-c946-49f6-99ef-ff4ab350a4c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cad3acc22b2eb44b3a116b77879253d7" ns2:_="">
     <xsd:import namespace="ffdfa1cc-c946-49f6-99ef-ff4ab350a4c7"/>
@@ -4087,12 +4397,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4103,6 +4407,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C84895-33C6-4EEF-ADE3-B2C6A0E7CE9B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FF34756-59E0-48B0-8E6C-773EF7EF3DA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4120,15 +4433,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C84895-33C6-4EEF-ADE3-B2C6A0E7CE9B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F33CB9-EBB9-4740-8AC2-6F0A2CE058F7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
update onTrack task files and worklogs
</commit_message>
<xml_diff>
--- a/Worklog.xlsx
+++ b/Worklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SIT723\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5E335D-E0F1-46E7-BD02-15A557D77E33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85E2638-848F-4C10-B61B-1379B35BFF18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D01C876E-0C57-1449-A864-F752FD507052}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="99">
   <si>
     <t>Student Name</t>
   </si>
@@ -311,6 +311,27 @@
   </si>
   <si>
     <t>Task 7.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conduct experiment using standard training and validation set (CBAM + ResNet, Adam,  learing rate 0.01, 0.001, 0.0001, 200 epochs) </t>
+  </si>
+  <si>
+    <t>Locate other dataset like: JAFFE and RAF</t>
+  </si>
+  <si>
+    <t>Tranform the images data to csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conduct experiment with JAFFE (CBAM + ResNet, SGD,  learing rate 0.01, 0.005, 0.001, 200 epochs) </t>
+  </si>
+  <si>
+    <t>Refine-tune experiment with FER2013 (try different batch size vs. learning rate)</t>
+  </si>
+  <si>
+    <t>Task 8.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conduct experiment with JAFFE (finetuning with optimizer, learning rate, epochs, batch size, network depth ...) </t>
   </si>
 </sst>
 </file>
@@ -748,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC54600-A529-144A-8AA1-058C0E013D1F}">
-  <dimension ref="A1:H254"/>
+  <dimension ref="A1:H249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D83" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+    <sheetView tabSelected="1" topLeftCell="C126" workbookViewId="0">
+      <selection activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3643,60 +3664,420 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D126" s="4"/>
+      <c r="A126" t="s">
+        <v>23</v>
+      </c>
+      <c r="B126" t="s">
+        <v>24</v>
+      </c>
+      <c r="C126" t="s">
+        <v>25</v>
+      </c>
+      <c r="D126" s="4">
+        <v>44445</v>
+      </c>
+      <c r="E126">
+        <v>120</v>
+      </c>
+      <c r="F126" t="s">
+        <v>20</v>
+      </c>
+      <c r="G126" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D127" s="4"/>
+      <c r="A127" t="s">
+        <v>23</v>
+      </c>
+      <c r="B127" t="s">
+        <v>24</v>
+      </c>
+      <c r="C127" t="s">
+        <v>25</v>
+      </c>
+      <c r="D127" s="4">
+        <v>44445</v>
+      </c>
+      <c r="E127">
+        <v>120</v>
+      </c>
+      <c r="F127" t="s">
+        <v>20</v>
+      </c>
+      <c r="G127" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D128" s="4"/>
-    </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D129" s="4"/>
-    </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D130" s="4"/>
-    </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D131" s="4"/>
-    </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D132" s="4"/>
-    </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D133" s="4"/>
-    </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D134" s="4"/>
-    </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D135" s="4"/>
-    </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D136" s="4"/>
-    </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D137" s="4"/>
-    </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D138" s="4"/>
-    </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D139" s="4"/>
-    </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D140" s="4"/>
-    </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D141" s="4"/>
-    </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D142" s="4"/>
-    </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D143" s="4"/>
-    </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>23</v>
+      </c>
+      <c r="B128" t="s">
+        <v>24</v>
+      </c>
+      <c r="C128" t="s">
+        <v>25</v>
+      </c>
+      <c r="D128" s="4">
+        <v>44446</v>
+      </c>
+      <c r="E128">
+        <v>120</v>
+      </c>
+      <c r="F128" t="s">
+        <v>20</v>
+      </c>
+      <c r="G128" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>23</v>
+      </c>
+      <c r="B129" t="s">
+        <v>24</v>
+      </c>
+      <c r="C129" t="s">
+        <v>25</v>
+      </c>
+      <c r="D129" s="4">
+        <v>44446</v>
+      </c>
+      <c r="E129">
+        <v>70</v>
+      </c>
+      <c r="F129" t="s">
+        <v>20</v>
+      </c>
+      <c r="G129" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>23</v>
+      </c>
+      <c r="B130" t="s">
+        <v>24</v>
+      </c>
+      <c r="C130" t="s">
+        <v>25</v>
+      </c>
+      <c r="D130" s="4">
+        <v>44448</v>
+      </c>
+      <c r="E130">
+        <v>100</v>
+      </c>
+      <c r="F130" t="s">
+        <v>12</v>
+      </c>
+      <c r="G130" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>23</v>
+      </c>
+      <c r="B131" t="s">
+        <v>24</v>
+      </c>
+      <c r="C131" t="s">
+        <v>25</v>
+      </c>
+      <c r="D131" s="4">
+        <v>44448</v>
+      </c>
+      <c r="E131">
+        <v>120</v>
+      </c>
+      <c r="F131" t="s">
+        <v>20</v>
+      </c>
+      <c r="G131" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>23</v>
+      </c>
+      <c r="B132" t="s">
+        <v>24</v>
+      </c>
+      <c r="C132" t="s">
+        <v>25</v>
+      </c>
+      <c r="D132" s="4">
+        <v>44448</v>
+      </c>
+      <c r="E132">
+        <v>60</v>
+      </c>
+      <c r="F132" t="s">
+        <v>20</v>
+      </c>
+      <c r="G132" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>23</v>
+      </c>
+      <c r="B133" t="s">
+        <v>24</v>
+      </c>
+      <c r="C133" t="s">
+        <v>25</v>
+      </c>
+      <c r="D133" s="4">
+        <v>44449</v>
+      </c>
+      <c r="E133">
+        <v>120</v>
+      </c>
+      <c r="F133" t="s">
+        <v>20</v>
+      </c>
+      <c r="G133" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>23</v>
+      </c>
+      <c r="B134" t="s">
+        <v>24</v>
+      </c>
+      <c r="C134" t="s">
+        <v>25</v>
+      </c>
+      <c r="D134" s="4">
+        <v>44449</v>
+      </c>
+      <c r="E134">
+        <v>120</v>
+      </c>
+      <c r="F134" t="s">
+        <v>20</v>
+      </c>
+      <c r="G134" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>23</v>
+      </c>
+      <c r="B135" t="s">
+        <v>24</v>
+      </c>
+      <c r="C135" t="s">
+        <v>25</v>
+      </c>
+      <c r="D135" s="4">
+        <v>44449</v>
+      </c>
+      <c r="E135">
+        <v>120</v>
+      </c>
+      <c r="F135" t="s">
+        <v>20</v>
+      </c>
+      <c r="G135" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>23</v>
+      </c>
+      <c r="B136" t="s">
+        <v>24</v>
+      </c>
+      <c r="C136" t="s">
+        <v>25</v>
+      </c>
+      <c r="D136" s="4">
+        <v>44450</v>
+      </c>
+      <c r="E136">
+        <v>120</v>
+      </c>
+      <c r="F136" t="s">
+        <v>20</v>
+      </c>
+      <c r="G136" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>23</v>
+      </c>
+      <c r="B137" t="s">
+        <v>24</v>
+      </c>
+      <c r="C137" t="s">
+        <v>25</v>
+      </c>
+      <c r="D137" s="4">
+        <v>44450</v>
+      </c>
+      <c r="E137">
+        <v>120</v>
+      </c>
+      <c r="F137" t="s">
+        <v>20</v>
+      </c>
+      <c r="G137" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>23</v>
+      </c>
+      <c r="B138" t="s">
+        <v>24</v>
+      </c>
+      <c r="C138" t="s">
+        <v>25</v>
+      </c>
+      <c r="D138" s="4">
+        <v>44450</v>
+      </c>
+      <c r="E138">
+        <v>70</v>
+      </c>
+      <c r="F138" t="s">
+        <v>20</v>
+      </c>
+      <c r="G138" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>23</v>
+      </c>
+      <c r="B139" t="s">
+        <v>24</v>
+      </c>
+      <c r="C139" t="s">
+        <v>25</v>
+      </c>
+      <c r="D139" s="4">
+        <v>44451</v>
+      </c>
+      <c r="E139">
+        <v>120</v>
+      </c>
+      <c r="F139" t="s">
+        <v>20</v>
+      </c>
+      <c r="G139" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>23</v>
+      </c>
+      <c r="B140" t="s">
+        <v>24</v>
+      </c>
+      <c r="C140" t="s">
+        <v>25</v>
+      </c>
+      <c r="D140" s="4">
+        <v>44451</v>
+      </c>
+      <c r="E140">
+        <v>120</v>
+      </c>
+      <c r="F140" t="s">
+        <v>20</v>
+      </c>
+      <c r="G140" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>23</v>
+      </c>
+      <c r="B141" t="s">
+        <v>24</v>
+      </c>
+      <c r="C141" t="s">
+        <v>25</v>
+      </c>
+      <c r="D141" s="4">
+        <v>44451</v>
+      </c>
+      <c r="E141">
+        <v>120</v>
+      </c>
+      <c r="F141" t="s">
+        <v>20</v>
+      </c>
+      <c r="G141" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>23</v>
+      </c>
+      <c r="B142" t="s">
+        <v>24</v>
+      </c>
+      <c r="C142" t="s">
+        <v>25</v>
+      </c>
+      <c r="D142" s="4">
+        <v>44451</v>
+      </c>
+      <c r="E142">
+        <v>90</v>
+      </c>
+      <c r="F142" t="s">
+        <v>20</v>
+      </c>
+      <c r="G142" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>23</v>
+      </c>
+      <c r="B143" t="s">
+        <v>24</v>
+      </c>
+      <c r="C143" t="s">
+        <v>25</v>
+      </c>
+      <c r="D143" s="4">
+        <v>44451</v>
+      </c>
+      <c r="E143">
+        <v>90</v>
+      </c>
+      <c r="F143" t="s">
+        <v>16</v>
+      </c>
+      <c r="G143" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D144" s="4"/>
     </row>
     <row r="145" spans="4:4" x14ac:dyDescent="0.25">
@@ -4013,21 +4394,6 @@
     </row>
     <row r="249" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D249" s="4"/>
-    </row>
-    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D250" s="4"/>
-    </row>
-    <row r="251" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D251" s="4"/>
-    </row>
-    <row r="252" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D252" s="4"/>
-    </row>
-    <row r="253" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D253" s="4"/>
-    </row>
-    <row r="254" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D254" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -4039,7 +4405,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E444</xm:sqref>
+          <xm:sqref>E3:E439</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A18E5B6F-7CCC-C74F-9785-6997C435583D}">
           <x14:formula1>
@@ -4058,7 +4424,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4190,8 +4556,14 @@
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="5">
+        <f>ROUNDDOWN(SUM(Logs!E126:E143)/60,0)</f>
+        <v>32</v>
+      </c>
+      <c r="C11" s="5">
+        <f>MOD(SUM(Logs!E126:E143),60)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -4219,11 +4591,11 @@
         <v>61</v>
       </c>
       <c r="B15" s="5">
-        <f>ROUNDDOWN(SUM(Logs!E3:E205)/60,0)</f>
-        <v>221</v>
+        <f>ROUNDDOWN(SUM(Logs!E3:E200)/60,0)</f>
+        <v>253</v>
       </c>
       <c r="C15" s="5">
-        <f>MOD(SUM(Logs!E3:E205),60)</f>
+        <f>MOD(SUM(Logs!E3:E200),60)</f>
         <v>50</v>
       </c>
     </row>
@@ -4352,6 +4724,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010082532935BEA4414DAD83A5DF5EC08D50" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1fab9b1b639c92c05cfd4aa2b4bf08c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffdfa1cc-c946-49f6-99ef-ff4ab350a4c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cad3acc22b2eb44b3a116b77879253d7" ns2:_="">
     <xsd:import namespace="ffdfa1cc-c946-49f6-99ef-ff4ab350a4c7"/>
@@ -4483,12 +4861,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4499,6 +4871,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C84895-33C6-4EEF-ADE3-B2C6A0E7CE9B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FF34756-59E0-48B0-8E6C-773EF7EF3DA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4516,15 +4897,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C84895-33C6-4EEF-ADE3-B2C6A0E7CE9B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F33CB9-EBB9-4740-8AC2-6F0A2CE058F7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
update worklogs and meeting minutes
</commit_message>
<xml_diff>
--- a/Worklog.xlsx
+++ b/Worklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SIT723\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B842726-BCEB-4FB4-AA94-85B4554814E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBD7A9E-1539-400B-A9DA-09A5C1FAA43B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D01C876E-0C57-1449-A864-F752FD507052}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D01C876E-0C57-1449-A864-F752FD507052}"/>
   </bookViews>
   <sheets>
     <sheet name="Logs" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="116">
   <si>
     <t>Student Name</t>
   </si>
@@ -377,6 +377,12 @@
   </si>
   <si>
     <t>Task 11.2 Research Handover</t>
+  </si>
+  <si>
+    <t>Task 12.2 learning summary</t>
+  </si>
+  <si>
+    <t>Task 12.1 Update the research report for final submission</t>
   </si>
 </sst>
 </file>
@@ -814,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC54600-A529-144A-8AA1-058C0E013D1F}">
-  <dimension ref="A1:H258"/>
+  <dimension ref="A1:H255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="C198" sqref="C198"/>
+    <sheetView topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="B206" sqref="B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5319,31 +5325,211 @@
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D196" s="4"/>
+      <c r="A196" t="s">
+        <v>23</v>
+      </c>
+      <c r="B196" t="s">
+        <v>24</v>
+      </c>
+      <c r="C196" t="s">
+        <v>25</v>
+      </c>
+      <c r="D196" s="4">
+        <v>44476</v>
+      </c>
+      <c r="E196">
+        <v>120</v>
+      </c>
+      <c r="F196" t="s">
+        <v>16</v>
+      </c>
+      <c r="G196" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D197" s="4"/>
+      <c r="A197" t="s">
+        <v>23</v>
+      </c>
+      <c r="B197" t="s">
+        <v>24</v>
+      </c>
+      <c r="C197" t="s">
+        <v>25</v>
+      </c>
+      <c r="D197" s="4">
+        <v>44476</v>
+      </c>
+      <c r="E197">
+        <v>20</v>
+      </c>
+      <c r="F197" t="s">
+        <v>16</v>
+      </c>
+      <c r="G197" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D198" s="4"/>
+      <c r="A198" t="s">
+        <v>23</v>
+      </c>
+      <c r="B198" t="s">
+        <v>24</v>
+      </c>
+      <c r="C198" t="s">
+        <v>25</v>
+      </c>
+      <c r="D198" s="4">
+        <v>44477</v>
+      </c>
+      <c r="E198">
+        <v>120</v>
+      </c>
+      <c r="F198" t="s">
+        <v>16</v>
+      </c>
+      <c r="G198" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D199" s="4"/>
+      <c r="A199" t="s">
+        <v>23</v>
+      </c>
+      <c r="B199" t="s">
+        <v>24</v>
+      </c>
+      <c r="C199" t="s">
+        <v>25</v>
+      </c>
+      <c r="D199" s="4">
+        <v>44477</v>
+      </c>
+      <c r="E199">
+        <v>80</v>
+      </c>
+      <c r="F199" t="s">
+        <v>16</v>
+      </c>
+      <c r="G199" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D200" s="4"/>
+      <c r="A200" t="s">
+        <v>23</v>
+      </c>
+      <c r="B200" t="s">
+        <v>24</v>
+      </c>
+      <c r="C200" t="s">
+        <v>25</v>
+      </c>
+      <c r="D200" s="4">
+        <v>44478</v>
+      </c>
+      <c r="E200">
+        <v>120</v>
+      </c>
+      <c r="F200" t="s">
+        <v>16</v>
+      </c>
+      <c r="G200" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D201" s="4"/>
+      <c r="A201" t="s">
+        <v>23</v>
+      </c>
+      <c r="B201" t="s">
+        <v>24</v>
+      </c>
+      <c r="C201" t="s">
+        <v>25</v>
+      </c>
+      <c r="D201" s="4">
+        <v>44478</v>
+      </c>
+      <c r="E201">
+        <v>120</v>
+      </c>
+      <c r="F201" t="s">
+        <v>16</v>
+      </c>
+      <c r="G201" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D202" s="4"/>
+      <c r="A202" t="s">
+        <v>23</v>
+      </c>
+      <c r="B202" t="s">
+        <v>24</v>
+      </c>
+      <c r="C202" t="s">
+        <v>25</v>
+      </c>
+      <c r="D202" s="4">
+        <v>44478</v>
+      </c>
+      <c r="E202">
+        <v>50</v>
+      </c>
+      <c r="F202" t="s">
+        <v>16</v>
+      </c>
+      <c r="G202" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D203" s="4"/>
+      <c r="A203" t="s">
+        <v>23</v>
+      </c>
+      <c r="B203" t="s">
+        <v>24</v>
+      </c>
+      <c r="C203" t="s">
+        <v>25</v>
+      </c>
+      <c r="D203" s="4">
+        <v>44479</v>
+      </c>
+      <c r="E203">
+        <v>120</v>
+      </c>
+      <c r="F203" t="s">
+        <v>16</v>
+      </c>
+      <c r="G203" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D204" s="4"/>
+      <c r="A204" t="s">
+        <v>23</v>
+      </c>
+      <c r="B204" t="s">
+        <v>24</v>
+      </c>
+      <c r="C204" t="s">
+        <v>25</v>
+      </c>
+      <c r="D204" s="4">
+        <v>44479</v>
+      </c>
+      <c r="E204">
+        <v>40</v>
+      </c>
+      <c r="F204" t="s">
+        <v>16</v>
+      </c>
+      <c r="G204" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D205" s="4"/>
@@ -5497,15 +5683,6 @@
     </row>
     <row r="255" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D255" s="4"/>
-    </row>
-    <row r="256" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D256" s="4"/>
-    </row>
-    <row r="257" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D257" s="4"/>
-    </row>
-    <row r="258" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D258" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -5517,7 +5694,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E448</xm:sqref>
+          <xm:sqref>E3:E445</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A18E5B6F-7CCC-C74F-9785-6997C435583D}">
           <x14:formula1>
@@ -5535,8 +5712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE2447B-8FF1-4200-A439-D9EB41D71D4F}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5720,20 +5897,26 @@
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="5">
+        <f>ROUNDDOWN(SUM(Logs!E196:E204)/60,0)</f>
+        <v>13</v>
+      </c>
+      <c r="C15" s="5">
+        <f>MOD(SUM(Logs!E196:E204),60)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B16" s="5">
-        <f>ROUNDDOWN(SUM(Logs!E3:E209)/60,0)</f>
-        <v>343</v>
+        <f>ROUNDDOWN(SUM(Logs!E3:E206)/60,0)</f>
+        <v>356</v>
       </c>
       <c r="C16" s="5">
-        <f>MOD(SUM(Logs!E3:E209),60)</f>
-        <v>20</v>
+        <f>MOD(SUM(Logs!E3:E206),60)</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -5861,6 +6044,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010082532935BEA4414DAD83A5DF5EC08D50" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1fab9b1b639c92c05cfd4aa2b4bf08c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffdfa1cc-c946-49f6-99ef-ff4ab350a4c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cad3acc22b2eb44b3a116b77879253d7" ns2:_="">
     <xsd:import namespace="ffdfa1cc-c946-49f6-99ef-ff4ab350a4c7"/>
@@ -5992,15 +6184,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6008,6 +6191,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F33CB9-EBB9-4740-8AC2-6F0A2CE058F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FF34756-59E0-48B0-8E6C-773EF7EF3DA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6025,14 +6216,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F33CB9-EBB9-4740-8AC2-6F0A2CE058F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C84895-33C6-4EEF-ADE3-B2C6A0E7CE9B}">
   <ds:schemaRefs>

</xml_diff>